<commit_message>
Act de base de datos
</commit_message>
<xml_diff>
--- a/Practicas/P2/Base_Libros_P2.xlsx
+++ b/Practicas/P2/Base_Libros_P2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/Mi unidad/Universidad/Ciencia de Datos/6to Semestre/2022_1-Base-Datos/Practicas/P2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C2014A-70D2-D046-B1E2-17BE8C2532A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4979D1C-9552-8546-B3DB-03A45B321BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9120" yWindow="500" windowWidth="19300" windowHeight="15900" xr2:uid="{1A9D2DCF-16A8-E540-93BA-8362006441DE}"/>
+    <workbookView xWindow="1520" yWindow="500" windowWidth="27280" windowHeight="15900" xr2:uid="{1A9D2DCF-16A8-E540-93BA-8362006441DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="101">
   <si>
     <t>membresia</t>
   </si>
@@ -215,6 +215,129 @@
   </si>
   <si>
     <t>fechnac</t>
+  </si>
+  <si>
+    <t>Suspenso</t>
+  </si>
+  <si>
+    <t>Fernando</t>
+  </si>
+  <si>
+    <t>Guillermo</t>
+  </si>
+  <si>
+    <t>Exhalation</t>
+  </si>
+  <si>
+    <t>1Q84</t>
+  </si>
+  <si>
+    <t>El coronel no tiene quien le escriba</t>
+  </si>
+  <si>
+    <t>El señor de las moscas</t>
+  </si>
+  <si>
+    <t>La maquina del tiempo</t>
+  </si>
+  <si>
+    <t>La guerra de los mundos</t>
+  </si>
+  <si>
+    <t>Bajo la rueda</t>
+  </si>
+  <si>
+    <t>Siddharta</t>
+  </si>
+  <si>
+    <t>El Lobo Estepario</t>
+  </si>
+  <si>
+    <t>One Shot</t>
+  </si>
+  <si>
+    <t>Ted Chiang</t>
+  </si>
+  <si>
+    <t>Haruki Murakami</t>
+  </si>
+  <si>
+    <t>Gabriel García Márquez</t>
+  </si>
+  <si>
+    <t>William Golding</t>
+  </si>
+  <si>
+    <t>H. G. Wells</t>
+  </si>
+  <si>
+    <t>Hermann Hesse</t>
+  </si>
+  <si>
+    <t>Lee Child</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrés </t>
+  </si>
+  <si>
+    <t>Urbano</t>
+  </si>
+  <si>
+    <t>Avitúa</t>
+  </si>
+  <si>
+    <t>Varela</t>
+  </si>
+  <si>
+    <t>Santa Rita</t>
+  </si>
+  <si>
+    <t>Vizuet</t>
+  </si>
+  <si>
+    <t>Yeudiel</t>
+  </si>
+  <si>
+    <t>Eduardo</t>
+  </si>
+  <si>
+    <t>Edgar</t>
+  </si>
+  <si>
+    <t>Harry Potter</t>
+  </si>
+  <si>
+    <t>On the road</t>
+  </si>
+  <si>
+    <t>The Pillars of the Earth</t>
+  </si>
+  <si>
+    <t>Fantasia</t>
+  </si>
+  <si>
+    <t>J. K. Rowling</t>
+  </si>
+  <si>
+    <t>Jack Kerouac</t>
+  </si>
+  <si>
+    <t>Ken Follett</t>
+  </si>
+  <si>
+    <t>Lara</t>
+  </si>
+  <si>
+    <t>Moreno</t>
+  </si>
+  <si>
+    <t>Callejas</t>
+  </si>
+  <si>
+    <t>Hernandez</t>
+  </si>
+  <si>
+    <t>Garduño</t>
   </si>
 </sst>
 </file>
@@ -247,12 +370,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -268,13 +397,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -590,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D824176F-40BF-604C-92E4-FC8528971DE1}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1202,43 +1337,565 @@
         <v>36622</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+    <row r="18" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
         <v>61683</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="6">
         <v>20</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="7">
         <v>2</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K18" s="4">
+      <c r="J18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="8">
         <v>36351</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J19" s="2"/>
+      <c r="A19" s="2">
+        <v>61685</v>
+      </c>
+      <c r="B19" s="2">
+        <v>21</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="2">
+        <v>4</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K19" s="10">
+        <v>35967</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>61686</v>
+      </c>
+      <c r="B20" s="2">
+        <v>22</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20" s="10">
+        <v>36111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>61686</v>
+      </c>
+      <c r="B21" s="2">
+        <v>23</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="2">
+        <v>4</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="10">
+        <v>36111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>61686</v>
+      </c>
+      <c r="B22" s="2">
+        <v>24</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="2">
+        <v>4</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" s="10">
+        <v>36111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>61686</v>
+      </c>
+      <c r="B23" s="2">
+        <v>25</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="2">
+        <v>4</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K23" s="10">
+        <v>36111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>61686</v>
+      </c>
+      <c r="B24" s="2">
+        <v>26</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="2">
+        <v>4</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K24" s="10">
+        <v>36111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>61687</v>
+      </c>
+      <c r="B25" s="2">
+        <v>27</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="2">
+        <v>4</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K25" s="10">
+        <v>32642</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>61687</v>
+      </c>
+      <c r="B26" s="2">
+        <v>28</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="2">
+        <v>5</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K26" s="10">
+        <v>32642</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>61687</v>
+      </c>
+      <c r="B27" s="2">
+        <v>29</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="2">
+        <v>5</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K27" s="10">
+        <v>32642</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>61687</v>
+      </c>
+      <c r="B28" s="2">
+        <v>30</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="2">
+        <v>4</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K28" s="10">
+        <v>32642</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>61687</v>
+      </c>
+      <c r="B29" s="2">
+        <v>20</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="2">
+        <v>4</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K29" s="10">
+        <v>32642</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>61688</v>
+      </c>
+      <c r="B30" s="2">
+        <v>31</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F30" s="2">
+        <v>5</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K30" s="10">
+        <v>36622</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>61689</v>
+      </c>
+      <c r="B31" s="2">
+        <v>30</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" s="2">
+        <v>5</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K31" s="10">
+        <v>36498</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>61685</v>
+      </c>
+      <c r="B32" s="2">
+        <v>33</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="2">
+        <v>5</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K32" s="10">
+        <v>35967</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>61690</v>
+      </c>
+      <c r="B33" s="2">
+        <v>34</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="2">
+        <v>4</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K33" s="10">
+        <v>37109</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>